<commit_message>
added mr and mrs in admin offic & updated phy excel
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/015.xlsx
+++ b/docs/STAFF-DATA/015.xlsx
@@ -5,22 +5,33 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1305D992-CC1D-48D1-A120-26737D916440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AA9CE4-1A38-44E3-A88E-62CD268D1C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15168" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -110,9 +121,6 @@
     <t>/static/images/profile_photos/015/VEC-015-04-091.webp</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.linkedin.com/in/hamsavalli-g-322069204/ </t>
-  </si>
-  <si>
     <t>VEC-015-04-091</t>
   </si>
   <si>
@@ -177,9 +185,6 @@
     <t xml:space="preserve">https://orcid.org/0009-0009-3888-9451 </t>
   </si>
   <si>
-    <t xml:space="preserve">MEK-9464-2025 </t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.scopus.com/authid/detail.uri?authorId=55816833000 </t>
   </si>
   <si>
@@ -245,9 +250,6 @@
     <t xml:space="preserve">https://www.scopus.com/authid/detail.uri?authorId=57710931100 </t>
   </si>
   <si>
-    <t xml:space="preserve">linkedin.com/in/sivatharani-boomiraja-54401b28b </t>
-  </si>
-  <si>
     <t>VEC-015-04-078</t>
   </si>
   <si>
@@ -261,13 +263,25 @@
   </si>
   <si>
     <t>Mr. RAVI KUMAR C</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0003-4302-6131</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/hamsavalli-g-322069204?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.webofscience.com/wos/author/record/MEK-9464-2025 </t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sivatharani-boomiraja-54401b28b/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +320,14 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -347,10 +369,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,8 +396,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -680,8 +707,8 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,12 +716,12 @@
     <col min="1" max="1" width="40.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="0.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="28.44140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
     <col min="8" max="8" width="3.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.44140625" style="6" customWidth="1"/>
     <col min="10" max="10" width="28.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -746,7 +773,7 @@
       <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -772,7 +799,9 @@
       <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="H3" s="3"/>
       <c r="I3" s="4" t="s">
         <v>23</v>
@@ -794,191 +823,197 @@
       <c r="D4" s="4"/>
       <c r="F4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" t="s">
         <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="F5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" t="s">
         <v>35</v>
-      </c>
-      <c r="J5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="J6" t="s">
         <v>51</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="J7" t="s">
         <v>43</v>
-      </c>
-      <c r="J7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="J8" t="s">
         <v>59</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="F9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="I10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" t="s">
         <v>70</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J10" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{A5F98899-F30B-4293-B019-034FEA9638D3}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{BF3A9B70-9AEA-4A70-B029-1A83F75D2D9D}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{AA2C6452-0B04-4D63-8947-AC1B393FE427}"/>
+    <hyperlink ref="I10" r:id="rId4" xr:uid="{5573DF8A-7AFD-4543-8377-2314489BC0B3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>